<commit_message>
Working on asserted_distribution batch preview.
</commit_message>
<xml_diff>
--- a/spec/files/batch/asserted_distribution/AssertedDistributionTest.xlsx
+++ b/spec/files/batch/asserted_distribution/AssertedDistributionTest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="37020" yWindow="2320" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="30340" yWindow="2920" windowWidth="25600" windowHeight="17560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,14 +19,38 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+  <si>
+    <t>otu_name</t>
+  </si>
+  <si>
+    <t>otu_id</t>
+  </si>
+  <si>
+    <t>geographic_area_name</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>county</t>
+  </si>
+  <si>
+    <t>source_id</t>
+  </si>
+  <si>
+    <t>doi</t>
+  </si>
+  <si>
+    <t>citation</t>
+  </si>
   <si>
     <t>Aus bus</t>
   </si>
   <si>
-    <t>Canada</t>
-  </si>
-  <si>
     <t>Saskatchewan</t>
   </si>
   <si>
@@ -36,62 +60,41 @@
     <t>Smith, 1920. Bears on the coast. Jr. Chilly Waters. 0:0 pp0-40.</t>
   </si>
   <si>
-    <t>otu_name</t>
-  </si>
-  <si>
-    <t>otu_id</t>
-  </si>
-  <si>
-    <t>geographic_area_name</t>
-  </si>
-  <si>
-    <t>country</t>
-  </si>
-  <si>
-    <t>state</t>
-  </si>
-  <si>
-    <t>county</t>
-  </si>
-  <si>
-    <t>source_id</t>
-  </si>
-  <si>
-    <t>doi</t>
-  </si>
-  <si>
-    <t>citation</t>
+    <t>Nebraska</t>
+  </si>
+  <si>
+    <t>Lincoln</t>
   </si>
   <si>
     <t>You must provide at least one of source_id, doi, citation, if more than provided priority of use is source_id, doi, then citation.</t>
   </si>
   <si>
-    <t>Omaha</t>
-  </si>
-  <si>
-    <t>USA</t>
-  </si>
-  <si>
-    <t>Nebraska</t>
-  </si>
-  <si>
-    <t>Lincoln</t>
-  </si>
-  <si>
-    <t>pilbert</t>
-  </si>
-  <si>
     <t>Chad</t>
   </si>
   <si>
     <t>philbert in Chad as described by Anon.</t>
+  </si>
+  <si>
+    <t>Aland</t>
+  </si>
+  <si>
+    <t>passive aggressive in Aland as described by Anon</t>
+  </si>
+  <si>
+    <t>Western Canada</t>
+  </si>
+  <si>
+    <t>philbert</t>
+  </si>
+  <si>
+    <t>United States</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -103,22 +106,6 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -141,35 +128,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="9">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -499,127 +476,144 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection sqref="A1:I5"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="4"/>
+    <col min="5" max="5" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="45">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:9" ht="30">
+      <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="F2" s="2"/>
+      <c r="G2" s="2">
         <v>11</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1">
-        <v>11</v>
-      </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:9" ht="105">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2">
         <v>7</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1" t="s">
-        <v>4</v>
+      <c r="C3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="195">
-      <c r="A4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1" t="s">
+      <c r="A4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="60">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2">
         <v>2</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1">
+      <c r="C5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2">
         <v>11</v>
       </c>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1" t="s">
-        <v>21</v>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="75">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2">
+        <v>10</v>
+      </c>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
More asserted_distribution test cases.
</commit_message>
<xml_diff>
--- a/spec/files/batch/asserted_distribution/AssertedDistributionTest.xlsx
+++ b/spec/files/batch/asserted_distribution/AssertedDistributionTest.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="27">
   <si>
     <t>otu_name</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>philbert in the United States as described by Anon.</t>
+  </si>
+  <si>
+    <t>Canada</t>
   </si>
 </sst>
 </file>
@@ -160,8 +163,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -195,7 +200,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -203,6 +208,7 @@
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -210,6 +216,7 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -539,10 +546,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -599,47 +606,43 @@
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:9" ht="105">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2">
+    <row r="3" spans="1:9">
+      <c r="A3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2">
+        <v>11</v>
+      </c>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+    </row>
+    <row r="4" spans="1:9" ht="105">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2">
         <v>7</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="195">
-      <c r="A4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="2">
-        <v>1</v>
-      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="75">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="195">
       <c r="A5" s="2" t="s">
         <v>21</v>
       </c>
@@ -651,16 +654,18 @@
       <c r="E5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="2"/>
+      <c r="F5" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="G5" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H5" s="2"/>
-      <c r="I5" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="60">
+      <c r="I5" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="75">
       <c r="A6" s="2" t="s">
         <v>21</v>
       </c>
@@ -669,16 +674,16 @@
       <c r="D6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="E6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="2"/>
       <c r="G6" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H6" s="2"/>
       <c r="I6" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="60">
@@ -687,38 +692,40 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="2" t="s">
-        <v>13</v>
-      </c>
+      <c r="D7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
         <v>14</v>
       </c>
       <c r="G7" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H7" s="2"/>
       <c r="I7" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="75">
+    <row r="8" spans="1:9" ht="60">
       <c r="A8" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
-      <c r="D8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="G8" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H8" s="2"/>
       <c r="I8" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="75">
@@ -727,73 +734,92 @@
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="2" t="s">
-        <v>13</v>
-      </c>
+      <c r="D9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="60">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="75">
       <c r="A10" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="3"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2" t="s">
+      <c r="E10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2">
+        <v>9</v>
+      </c>
+      <c r="H10" s="2"/>
+      <c r="I10" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="60">
+      <c r="A11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G11" s="2">
         <v>10</v>
-      </c>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="60">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2">
-        <v>2</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2">
-        <v>11</v>
       </c>
       <c r="H11" s="2"/>
       <c r="I11" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="75">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="60">
       <c r="A12" s="2"/>
       <c r="B12" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H12" s="2"/>
       <c r="I12" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="75">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2">
+        <v>1</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2">
+        <v>10</v>
+      </c>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
More work for geometery-less feature.
</commit_message>
<xml_diff>
--- a/spec/files/batch/asserted_distribution/AssertedDistributionTest.xlsx
+++ b/spec/files/batch/asserted_distribution/AssertedDistributionTest.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="29">
   <si>
     <t>otu_name</t>
   </si>
@@ -103,6 +103,9 @@
   </si>
   <si>
     <t>albert</t>
+  </si>
+  <si>
+    <t>Aus aus</t>
   </si>
 </sst>
 </file>
@@ -166,8 +169,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -205,7 +210,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="21">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -215,6 +220,7 @@
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -224,6 +230,7 @@
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -553,10 +560,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:XFD15"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -660,41 +667,37 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
+    <row r="6" spans="1:9" ht="105">
+      <c r="A6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="2">
+        <v>8</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-    </row>
-    <row r="7" spans="1:9" ht="195">
-      <c r="A7" s="2" t="s">
-        <v>21</v>
-      </c>
+      <c r="I6" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
-      <c r="D7" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" s="2">
-        <v>1</v>
-      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
       <c r="H7" s="2"/>
-      <c r="I7" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="75">
+      <c r="I7" s="2"/>
+    </row>
+    <row r="8" spans="1:9" ht="195">
       <c r="A8" s="2" t="s">
         <v>21</v>
       </c>
@@ -706,16 +709,18 @@
       <c r="E8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="2"/>
+      <c r="F8" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="G8" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H8" s="2"/>
-      <c r="I8" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="60">
+      <c r="I8" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="75">
       <c r="A9" s="2" t="s">
         <v>21</v>
       </c>
@@ -724,16 +729,16 @@
       <c r="D9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="E9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="2"/>
       <c r="G9" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="60">
@@ -742,38 +747,40 @@
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="2" t="s">
-        <v>13</v>
-      </c>
+      <c r="D10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="2"/>
       <c r="F10" s="2" t="s">
         <v>14</v>
       </c>
       <c r="G10" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H10" s="2"/>
       <c r="I10" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="75">
+    <row r="11" spans="1:9" ht="60">
       <c r="A11" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
-      <c r="D11" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="G11" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H11" s="2"/>
       <c r="I11" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="75">
@@ -782,22 +789,22 @@
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="2" t="s">
-        <v>13</v>
-      </c>
+      <c r="D12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="H12" s="2"/>
       <c r="I12" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="75">
       <c r="A13" s="2" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -806,77 +813,96 @@
         <v>13</v>
       </c>
       <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
+      <c r="G13" s="2">
+        <v>9</v>
+      </c>
       <c r="H13" s="2"/>
       <c r="I13" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="60">
+    <row r="14" spans="1:9" ht="75">
       <c r="A14" s="2" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="3"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G14" s="2">
-        <v>10</v>
-      </c>
+      <c r="E14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
       <c r="H14" s="2"/>
-      <c r="I14" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="A15" s="2"/>
+      <c r="I14" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="60">
+      <c r="A15" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="3"/>
       <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
+      <c r="F15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15" s="2">
+        <v>10</v>
+      </c>
       <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-    </row>
-    <row r="16" spans="1:9" ht="60">
+      <c r="I15" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16" s="2"/>
-      <c r="B16" s="2">
-        <v>2</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="3"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
-      <c r="G16" s="2">
-        <v>11</v>
-      </c>
+      <c r="G16" s="2"/>
       <c r="H16" s="2"/>
-      <c r="I16" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="75">
+      <c r="I16" s="2"/>
+    </row>
+    <row r="17" spans="1:9" ht="60">
       <c r="A17" s="2"/>
       <c r="B17" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H17" s="2"/>
       <c r="I17" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="75">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2">
+        <v>1</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2">
+        <v>10</v>
+      </c>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>